<commit_message>
updated schematic pdf and bom
</commit_message>
<xml_diff>
--- a/PCB/LightShaker-3 - MAX1765_hotFix/LightShaker-3_BOM.xlsx
+++ b/PCB/LightShaker-3 - MAX1765_hotFix/LightShaker-3_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SteDun00\Desktop\GitHub\PCB\LightShaker-3 - MAX1765_hotFix\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\LightShaker\PCB\LightShaker-3 - MAX1765_hotFix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578769F0-7F5C-4E46-BB16-EF0ADF63F0A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC22E65-935E-412E-B5A0-66887DF93E1C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38220" yWindow="1695" windowWidth="35265" windowHeight="18030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LightShaker-3" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="73">
   <si>
     <t>LightShaker-3</t>
   </si>
@@ -234,9 +234,6 @@
     <t>SK9822</t>
   </si>
   <si>
-    <t>R1, R4, R9, R10, R11, R15, R18</t>
-  </si>
-  <si>
     <t>SMD LED</t>
   </si>
   <si>
@@ -247,6 +244,15 @@
   </si>
   <si>
     <t>58um transparent foil</t>
+  </si>
+  <si>
+    <t>39k</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>R1, R4, R9, R11, R15, R18</t>
   </si>
 </sst>
 </file>
@@ -1159,10 +1165,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,7 +1191,7 @@
         <v>61</v>
       </c>
       <c r="E1">
-        <f>B4+B6+B5+B7+B8+B9+B10+B11+B12+B13+B14+B15+B16+B17+B18+B19+B20+B21+B22</f>
+        <f>B4+B6+B5+B7+B8+B9+B10+B11+B13+B14+B15+B16+B17+B18+B19+B20+B21+B22+B23</f>
         <v>64</v>
       </c>
     </row>
@@ -1369,10 +1375,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>11</v>
@@ -1381,7 +1387,7 @@
         <v>12</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>13</v>
@@ -1389,117 +1395,119 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="2">
         <v>3</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="2">
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="2">
         <v>16</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="2">
-        <v>3</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="G16" s="2" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G17" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
         <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G18" s="2"/>
     </row>
@@ -1508,16 +1516,16 @@
         <v>1</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G19" s="2"/>
     </row>
@@ -1526,87 +1534,105 @@
         <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>60</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="G20" s="2"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
+        <v>3</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="2">
         <v>1</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="5" t="s">
+      <c r="G23" s="2"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="2">
+        <v>1</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="2">
-        <v>1</v>
-      </c>
-      <c r="C27" s="6" t="s">
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="C28:F28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>